<commit_message>
DATA: Combine NABD and TU datasets into table for geospatial/connectivity processing
</commit_message>
<xml_diff>
--- a/Data/TU/TU_BearLake.xlsx
+++ b/Data/TU/TU_BearLake.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://troutunlimited11-my.sharepoint.com/personal/james_derito_tu_org/Documents/Documents/TU2/Fish Passage/Fish passage connectivity_Greg Goodrum/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a02290896\Downloads\TU-BRLC_Barriers\Data\TU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="214" documentId="13_ncr:1_{2827D87A-A07A-45AE-B137-601B371EC081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FC34583-9531-443C-9C7F-93AE85DFBAAD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FC01C6-2ABC-4D73-99B6-61D219A608BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diversions" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,9 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId4"/>
-    <pivotCache cacheId="5" r:id="rId5"/>
-    <pivotCache cacheId="6" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
+    <pivotCache cacheId="2" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -167,7 +167,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="251">
   <si>
     <t>St. Charles Creek</t>
   </si>
@@ -917,6 +917,9 @@
   </si>
   <si>
     <t xml:space="preserve">Diversion was rebuilt in 2022 with a new headgate diversion structure. The intent is to install a fish screen in canal. That hasn't occurred yet. </t>
+  </si>
+  <si>
+    <t>CUL_ID</t>
   </si>
 </sst>
 </file>
@@ -924,8 +927,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.000000"/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -1482,7 +1485,7 @@
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1507,7 +1510,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1550,23 +1553,22 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1575,15 +1577,14 @@
     <xf numFmtId="0" fontId="1" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5196,7 +5197,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3BFFDA04-A0B8-4C55-A415-EA0137425679}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3BFFDA04-A0B8-4C55-A415-EA0137425679}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="O38:P45" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -5256,7 +5257,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F5DDB253-EEAD-4BCE-9DD0-0D3C860F9B3C}" name="PivotTable8" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F5DDB253-EEAD-4BCE-9DD0-0D3C860F9B3C}" name="PivotTable8" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="U28:V50" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -5376,7 +5377,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{613487E3-E6C3-4B37-B09A-7AC82010E0BD}" name="PivotTable7" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{613487E3-E6C3-4B37-B09A-7AC82010E0BD}" name="PivotTable7" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="Z28:AA45" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -5764,8 +5765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5793,16 +5794,16 @@
       <c r="A1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="33" t="s">
         <v>110</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="34" t="s">
         <v>34</v>
       </c>
       <c r="F1" s="18" t="s">
@@ -5811,10 +5812,10 @@
       <c r="G1" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="35" t="s">
         <v>119</v>
       </c>
       <c r="J1" s="20" t="s">
@@ -5835,10 +5836,10 @@
       <c r="O1" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="P1" s="37" t="s">
+      <c r="P1" s="36" t="s">
         <v>236</v>
       </c>
-      <c r="Q1" s="37" t="s">
+      <c r="Q1" s="36" t="s">
         <v>235</v>
       </c>
       <c r="R1" s="20" t="s">
@@ -5852,16 +5853,16 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="30" t="s">
         <v>41</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D2" s="32">
+      <c r="D2" s="31">
         <v>42.036247000000003</v>
       </c>
-      <c r="E2" s="32">
+      <c r="E2" s="31">
         <v>-111.404307</v>
       </c>
       <c r="F2" t="s">
@@ -5894,10 +5895,10 @@
       <c r="O2" s="3">
         <v>2008</v>
       </c>
-      <c r="P2" s="42">
+      <c r="P2" s="40">
         <v>1</v>
       </c>
-      <c r="Q2" s="42">
+      <c r="Q2" s="40">
         <v>1</v>
       </c>
       <c r="R2" s="3" t="s">
@@ -5911,16 +5912,16 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="30" t="s">
         <v>42</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D3" s="32">
+      <c r="D3" s="31">
         <v>42.036574000000002</v>
       </c>
-      <c r="E3" s="32">
+      <c r="E3" s="31">
         <v>-111.4081</v>
       </c>
       <c r="F3" t="s">
@@ -5953,10 +5954,10 @@
       <c r="O3" s="3">
         <v>2008</v>
       </c>
-      <c r="P3" s="42">
+      <c r="P3" s="40">
         <v>1</v>
       </c>
-      <c r="Q3" s="42">
+      <c r="Q3" s="40">
         <v>1</v>
       </c>
       <c r="R3" s="3" t="s">
@@ -5970,16 +5971,16 @@
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="30" t="s">
         <v>43</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="31">
         <v>42.036476</v>
       </c>
-      <c r="E4" s="32">
+      <c r="E4" s="31">
         <v>-111.410741</v>
       </c>
       <c r="F4" t="s">
@@ -6012,10 +6013,10 @@
       <c r="O4" s="3">
         <v>2008</v>
       </c>
-      <c r="P4" s="42">
+      <c r="P4" s="40">
         <v>1</v>
       </c>
-      <c r="Q4" s="42">
+      <c r="Q4" s="40">
         <v>1</v>
       </c>
       <c r="R4" s="3" t="s">
@@ -6029,16 +6030,16 @@
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="30" t="s">
         <v>45</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="32">
+      <c r="D5" s="31">
         <v>42.040250999999998</v>
       </c>
-      <c r="E5" s="32">
+      <c r="E5" s="31">
         <v>-111.429603</v>
       </c>
       <c r="F5" t="s">
@@ -6071,10 +6072,10 @@
       <c r="O5" s="3">
         <v>2008</v>
       </c>
-      <c r="P5" s="42">
+      <c r="P5" s="40">
         <v>1</v>
       </c>
-      <c r="Q5" s="42">
+      <c r="Q5" s="40">
         <v>1</v>
       </c>
       <c r="R5" s="3" t="s">
@@ -6088,16 +6089,16 @@
       <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="30" t="s">
         <v>46</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D6" s="31">
         <v>42.041127000000003</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="31">
         <v>-111.43320300000001</v>
       </c>
       <c r="F6" t="s">
@@ -6130,10 +6131,10 @@
       <c r="O6" s="3">
         <v>2008</v>
       </c>
-      <c r="P6" s="42">
+      <c r="P6" s="40">
         <v>1</v>
       </c>
-      <c r="Q6" s="42">
+      <c r="Q6" s="40">
         <v>1</v>
       </c>
       <c r="R6" s="3" t="s">
@@ -6147,16 +6148,16 @@
       <c r="A7" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="30" t="s">
         <v>49</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="31">
         <v>42.122883999999999</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="31">
         <v>-111.3361</v>
       </c>
       <c r="F7" t="s">
@@ -6189,10 +6190,10 @@
       <c r="O7" s="3">
         <v>1995</v>
       </c>
-      <c r="P7" s="42">
+      <c r="P7" s="40">
         <v>0</v>
       </c>
-      <c r="Q7" s="42">
+      <c r="Q7" s="40">
         <v>1</v>
       </c>
       <c r="R7" s="3" t="s">
@@ -6206,16 +6207,16 @@
       <c r="A8" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="30" t="s">
         <v>50</v>
       </c>
       <c r="C8" t="s">
         <v>98</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="31">
         <v>42.139789999999998</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="31">
         <v>-111.36490999999999</v>
       </c>
       <c r="F8" t="s">
@@ -6248,10 +6249,10 @@
       <c r="O8" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="P8" s="42">
+      <c r="P8" s="40">
         <v>0.8</v>
       </c>
-      <c r="Q8" s="42">
+      <c r="Q8" s="40">
         <v>0.8</v>
       </c>
       <c r="R8" s="3" t="s">
@@ -6265,16 +6266,16 @@
       <c r="A9" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="30" t="s">
         <v>51</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="32">
+      <c r="D9" s="31">
         <v>42.124470000000002</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="31">
         <v>-111.389627</v>
       </c>
       <c r="F9" t="s">
@@ -6307,10 +6308,10 @@
       <c r="O9" s="3">
         <v>1999</v>
       </c>
-      <c r="P9" s="42">
+      <c r="P9" s="40">
         <v>0.8</v>
       </c>
-      <c r="Q9" s="42">
+      <c r="Q9" s="40">
         <v>1</v>
       </c>
       <c r="R9" s="3" t="s">
@@ -6324,16 +6325,16 @@
       <c r="A10" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="30" t="s">
         <v>52</v>
       </c>
       <c r="C10" t="s">
         <v>100</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="31">
         <v>42.115619000000002</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="31">
         <v>-111.369371</v>
       </c>
       <c r="F10" t="s">
@@ -6363,10 +6364,10 @@
       <c r="N10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="P10" s="42">
+      <c r="P10" s="40">
         <v>0.8</v>
       </c>
-      <c r="Q10" s="42">
+      <c r="Q10" s="40">
         <v>0.8</v>
       </c>
       <c r="R10" s="3" t="s">
@@ -6380,16 +6381,16 @@
       <c r="A11" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="30" t="s">
         <v>99</v>
       </c>
       <c r="C11" t="s">
         <v>102</v>
       </c>
-      <c r="D11" s="32">
+      <c r="D11" s="31">
         <v>42.119148000000003</v>
       </c>
-      <c r="E11" s="32">
+      <c r="E11" s="31">
         <v>-111.385017</v>
       </c>
       <c r="F11" t="s">
@@ -6422,10 +6423,10 @@
       <c r="O11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="P11" s="42">
+      <c r="P11" s="40">
         <v>1</v>
       </c>
-      <c r="Q11" s="42">
+      <c r="Q11" s="40">
         <v>1</v>
       </c>
       <c r="R11" s="3" t="s">
@@ -6439,16 +6440,16 @@
       <c r="A12" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="30" t="s">
         <v>101</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="32">
+      <c r="D12" s="31">
         <v>42.121327000000001</v>
       </c>
-      <c r="E12" s="32">
+      <c r="E12" s="31">
         <v>-111.414644</v>
       </c>
       <c r="F12" t="s">
@@ -6481,10 +6482,10 @@
       <c r="O12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="P12" s="42">
+      <c r="P12" s="40">
         <v>1</v>
       </c>
-      <c r="Q12" s="42">
+      <c r="Q12" s="40">
         <v>1</v>
       </c>
       <c r="R12" s="3" t="s">
@@ -6498,16 +6499,16 @@
       <c r="A13" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="30" t="s">
         <v>245</v>
       </c>
       <c r="C13" t="s">
         <v>246</v>
       </c>
-      <c r="D13" s="32">
+      <c r="D13" s="31">
         <v>42.120866999999997</v>
       </c>
-      <c r="E13" s="32">
+      <c r="E13" s="31">
         <v>-111.418644</v>
       </c>
       <c r="F13" t="s">
@@ -6540,10 +6541,10 @@
       <c r="O13" s="3">
         <v>2022</v>
       </c>
-      <c r="P13" s="42">
+      <c r="P13" s="40">
         <v>0.95</v>
       </c>
-      <c r="Q13" s="42">
+      <c r="Q13" s="40">
         <v>0.95</v>
       </c>
       <c r="R13" s="3" t="s">
@@ -6557,16 +6558,16 @@
       <c r="A14" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="30" t="s">
         <v>103</v>
       </c>
       <c r="C14" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="32">
+      <c r="D14" s="31">
         <v>42.115105</v>
       </c>
-      <c r="E14" s="32">
+      <c r="E14" s="31">
         <v>-111.440657</v>
       </c>
       <c r="F14" t="s">
@@ -6599,10 +6600,10 @@
       <c r="O14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="P14" s="42">
+      <c r="P14" s="40">
         <v>1</v>
       </c>
-      <c r="Q14" s="42">
+      <c r="Q14" s="40">
         <v>1</v>
       </c>
       <c r="R14" s="3" t="s">
@@ -6616,16 +6617,16 @@
       <c r="A15" t="s">
         <v>207</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="30" t="s">
         <v>208</v>
       </c>
       <c r="C15" t="s">
         <v>213</v>
       </c>
-      <c r="D15" s="32">
+      <c r="D15" s="31">
         <v>41.984859999999998</v>
       </c>
-      <c r="E15" s="32">
+      <c r="E15" s="31">
         <v>-111.415888</v>
       </c>
       <c r="F15" t="s">
@@ -6658,10 +6659,10 @@
       <c r="O15" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="P15" s="42">
+      <c r="P15" s="40">
         <v>1</v>
       </c>
-      <c r="Q15" s="42">
+      <c r="Q15" s="40">
         <v>1</v>
       </c>
       <c r="R15" s="3" t="s">
@@ -6675,16 +6676,16 @@
       <c r="A16" t="s">
         <v>222</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="30" t="s">
         <v>223</v>
       </c>
       <c r="C16" t="s">
         <v>224</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D16" s="31">
         <v>41.986776999999996</v>
       </c>
-      <c r="E16" s="32">
+      <c r="E16" s="31">
         <v>-111.245935</v>
       </c>
       <c r="F16" t="s">
@@ -6717,11 +6718,11 @@
       <c r="O16" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="P16" s="42">
-        <v>0.5</v>
-      </c>
-      <c r="Q16" s="42" t="s">
-        <v>24</v>
+      <c r="P16" s="40">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="40">
+        <v>0</v>
       </c>
       <c r="R16" s="3" t="s">
         <v>9</v>
@@ -6819,31 +6820,31 @@
       <c r="A1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="33" t="s">
         <v>111</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="35" t="s">
         <v>37</v>
       </c>
       <c r="K1" s="20" t="s">
@@ -6870,10 +6871,10 @@
       <c r="R1" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="S1" s="40" t="s">
+      <c r="S1" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="T1" s="40" t="s">
+      <c r="T1" s="38" t="s">
         <v>94</v>
       </c>
       <c r="U1" s="20" t="s">
@@ -6888,7 +6889,7 @@
       <c r="X1" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="Y1" s="40" t="s">
+      <c r="Y1" s="38" t="s">
         <v>86</v>
       </c>
       <c r="Z1" s="21" t="s">
@@ -6966,19 +6967,19 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="30" t="s">
         <v>41</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
       </c>
-      <c r="E2" s="30">
+      <c r="E2" s="29">
         <v>42.036284999999999</v>
       </c>
-      <c r="F2" s="30">
+      <c r="F2" s="29">
         <v>-111.404242</v>
       </c>
       <c r="G2" t="s">
@@ -7109,19 +7110,19 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="30" t="s">
         <v>42</v>
       </c>
       <c r="D3" s="2">
         <v>3</v>
       </c>
-      <c r="E3" s="30">
+      <c r="E3" s="29">
         <v>42.036557000000002</v>
       </c>
-      <c r="F3" s="30">
+      <c r="F3" s="29">
         <v>-111.40806499999999</v>
       </c>
       <c r="G3" t="s">
@@ -7249,19 +7250,19 @@
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="30" t="s">
         <v>43</v>
       </c>
       <c r="D4" s="2">
         <v>2</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="29">
         <v>42.036378999999997</v>
       </c>
-      <c r="F4" s="30">
+      <c r="F4" s="29">
         <v>-111.410616</v>
       </c>
       <c r="G4" t="s">
@@ -7392,19 +7393,19 @@
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="30" t="s">
         <v>45</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="29">
         <v>42.040221000000003</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5" s="29">
         <v>-111.42951100000001</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -7538,19 +7539,19 @@
       <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="30" t="s">
         <v>46</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="29">
         <v>42.041113000000003</v>
       </c>
-      <c r="F6" s="30">
+      <c r="F6" s="29">
         <v>-111.43318600000001</v>
       </c>
       <c r="G6" s="2" t="s">
@@ -7681,19 +7682,19 @@
       <c r="A7" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="30" t="s">
         <v>113</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="29">
         <v>42.125388496600003</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F7" s="29">
         <v>-111.338484467</v>
       </c>
       <c r="G7" t="s">
@@ -7824,19 +7825,19 @@
       <c r="A8" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="30" t="s">
         <v>114</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E8" s="30">
+      <c r="E8" s="29">
         <v>42.130368745699897</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8" s="29">
         <v>-111.341008477</v>
       </c>
       <c r="G8" t="s">
@@ -7967,19 +7968,19 @@
       <c r="A9" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="30" t="s">
         <v>115</v>
       </c>
       <c r="D9" t="s">
         <v>117</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9" s="29">
         <v>42.144517999999998</v>
       </c>
-      <c r="F9" s="30">
+      <c r="F9" s="29">
         <v>-111.36858700000001</v>
       </c>
       <c r="G9" t="s">
@@ -8107,19 +8108,19 @@
       <c r="A10" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="30" t="s">
         <v>116</v>
       </c>
       <c r="D10" t="s">
         <v>118</v>
       </c>
-      <c r="E10" s="30">
+      <c r="E10" s="29">
         <v>42.145327999999999</v>
       </c>
-      <c r="F10" s="30">
+      <c r="F10" s="29">
         <v>-111.37219899999999</v>
       </c>
       <c r="G10" t="s">
@@ -8236,19 +8237,19 @@
       <c r="A11" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="30" t="s">
         <v>51</v>
       </c>
       <c r="D11" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="30">
+      <c r="E11" s="29">
         <v>42.124408000000003</v>
       </c>
-      <c r="F11" s="30">
+      <c r="F11" s="29">
         <v>-111.389612</v>
       </c>
       <c r="G11" t="s">
@@ -8379,19 +8380,19 @@
       <c r="A12" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="30" t="s">
         <v>52</v>
       </c>
       <c r="D12" t="s">
         <v>100</v>
       </c>
-      <c r="E12" s="30">
+      <c r="E12" s="29">
         <v>42.115870999999999</v>
       </c>
-      <c r="F12" s="30">
+      <c r="F12" s="29">
         <v>-111.36894700000001</v>
       </c>
       <c r="G12" t="s">
@@ -8525,19 +8526,19 @@
       <c r="A13" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" t="s">
         <v>99</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="30" t="s">
         <v>99</v>
       </c>
       <c r="D13" t="s">
         <v>102</v>
       </c>
-      <c r="E13" s="30">
+      <c r="E13" s="29">
         <v>42.119163</v>
       </c>
-      <c r="F13" s="30">
+      <c r="F13" s="29">
         <v>-111.385035</v>
       </c>
       <c r="G13" t="s">
@@ -8662,19 +8663,19 @@
       <c r="A14" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="30" t="s">
         <v>101</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="30">
+      <c r="E14" s="29">
         <v>42.121231000000002</v>
       </c>
-      <c r="F14" s="30">
+      <c r="F14" s="29">
         <v>-111.413218</v>
       </c>
       <c r="G14" t="s">
@@ -8793,19 +8794,19 @@
       <c r="A15" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" t="s">
         <v>103</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="30" t="s">
         <v>103</v>
       </c>
       <c r="D15" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="30">
+      <c r="E15" s="29">
         <v>42.115045000000002</v>
       </c>
-      <c r="F15" s="30">
+      <c r="F15" s="29">
         <v>-111.440414</v>
       </c>
       <c r="G15" t="s">
@@ -8924,19 +8925,19 @@
       <c r="A16" t="s">
         <v>207</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B16" t="s">
         <v>208</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="30" t="s">
         <v>208</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="E16" s="30">
+      <c r="E16" s="29">
         <v>41.984743000000002</v>
       </c>
-      <c r="F16" s="30">
+      <c r="F16" s="29">
         <v>-111.415721</v>
       </c>
       <c r="G16" t="s">
@@ -9603,150 +9604,165 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A3F4D6A-83BC-4D1D-9AE7-A96414CE1F8D}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" style="2" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" style="3" customWidth="1"/>
-    <col min="4" max="5" width="25.28515625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="28" style="3" customWidth="1"/>
-    <col min="7" max="7" width="29.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="19" style="2" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" style="3" customWidth="1"/>
+    <col min="5" max="6" width="25.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="28" style="3" customWidth="1"/>
+    <col min="8" max="8" width="29.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="21" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="21" t="s">
+        <v>250</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>228</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="D1" s="39" t="s">
         <v>229</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="E1" s="39" t="s">
         <v>230</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="F1" s="39" t="s">
         <v>241</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="G1" s="19" t="s">
         <v>231</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="H1" s="19" t="s">
         <v>234</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="I1" s="35" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
         <v>222</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="C2" s="3">
+      <c r="D2" s="3">
         <v>41.987087000000002</v>
       </c>
-      <c r="D2" s="3">
+      <c r="E2" s="3">
         <v>-111.264433</v>
       </c>
-      <c r="E2" s="3">
+      <c r="F2" s="3">
         <v>2025</v>
       </c>
-      <c r="F2" s="33">
+      <c r="G2" s="32">
         <v>0</v>
       </c>
-      <c r="G2" s="3">
+      <c r="H2" s="3">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="C3" s="3">
+      <c r="D3" s="3">
         <v>42.034737999999997</v>
       </c>
-      <c r="D3" s="3">
+      <c r="E3" s="3">
         <v>-111.39516</v>
       </c>
-      <c r="E3" s="3">
+      <c r="F3" s="3">
         <v>2009</v>
       </c>
-      <c r="F3" s="33">
+      <c r="G3" s="32">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="G3" s="3">
+      <c r="H3" s="3">
         <v>1</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="C4" s="3">
+      <c r="D4" s="3">
         <v>42.03501</v>
       </c>
-      <c r="D4" s="3">
+      <c r="E4" s="3">
         <v>-111.396151</v>
       </c>
-      <c r="E4" s="3">
+      <c r="F4" s="3">
         <v>2014</v>
       </c>
-      <c r="F4" s="33">
+      <c r="G4" s="32">
         <v>0.95</v>
       </c>
-      <c r="G4" s="3">
+      <c r="H4" s="3">
         <v>1</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="C5" s="3">
+      <c r="D5" s="3">
         <v>42.053041999999998</v>
       </c>
-      <c r="D5" s="3">
+      <c r="E5" s="3">
         <v>-111.461287</v>
       </c>
-      <c r="E5" s="3">
+      <c r="F5" s="3">
         <v>2014</v>
       </c>
-      <c r="F5" s="33">
+      <c r="G5" s="32">
         <v>0.9</v>
       </c>
-      <c r="G5" s="3">
+      <c r="H5" s="3">
         <v>1</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>244</v>
       </c>
     </row>

</xml_diff>